<commit_message>
Need to validate grouping of bird point counts
updated excel with guess of changes (sheet 1 of bird_data_independent_reps.xlsx)
</commit_message>
<xml_diff>
--- a/data/bird_data_independent reps.xlsx
+++ b/data/bird_data_independent reps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\Projects\Mangrove restoration\birds_grenada_mangroves\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jodydaniel/OneDrive/Coding Projects/Gaea Conservation Network/ECCC/birds_grenada_mangroves/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E17CFA1B-CE0D-487B-BB38-FD5DF2BFD135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F348167-BF9E-0C4F-B218-8206A5174D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="1710" windowWidth="26175" windowHeight="14295" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="14300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bird_data_independent reps" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="113">
   <si>
     <t>Site</t>
   </si>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1218,37 +1218,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S244"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -6951,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -7693,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -7905,7 +7905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>48</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>48</v>
       </c>
@@ -8594,7 +8594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>48</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>48</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>48</v>
       </c>
@@ -8753,7 +8753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>48</v>
       </c>
@@ -8806,7 +8806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>48</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>48</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>48</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>48</v>
       </c>
@@ -9018,7 +9018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>48</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>48</v>
       </c>
@@ -9124,7 +9124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>48</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>48</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>48</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>79</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>79</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>79</v>
       </c>
@@ -9459,7 +9459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>79</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>79</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>79</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>79</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>79</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>79</v>
       </c>
@@ -9705,7 +9705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>79</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>79</v>
       </c>
@@ -9790,7 +9790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>79</v>
       </c>
@@ -9834,7 +9834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>79</v>
       </c>
@@ -9878,7 +9878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>79</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>79</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>79</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>79</v>
       </c>
@@ -10054,7 +10054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>79</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>79</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>79</v>
       </c>
@@ -10183,7 +10183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>79</v>
       </c>
@@ -10224,7 +10224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>79</v>
       </c>
@@ -10265,7 +10265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>79</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>79</v>
       </c>
@@ -10350,7 +10350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>79</v>
       </c>
@@ -10394,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>79</v>
       </c>
@@ -10438,7 +10438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>79</v>
       </c>
@@ -10482,7 +10482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>79</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>79</v>
       </c>
@@ -10570,7 +10570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>79</v>
       </c>
@@ -10614,7 +10614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>79</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>79</v>
       </c>
@@ -10702,7 +10702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>91</v>
       </c>
@@ -10743,7 +10743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>91</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>91</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>91</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>91</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>91</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>91</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>91</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>91</v>
       </c>
@@ -11071,7 +11071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>91</v>
       </c>
@@ -11112,7 +11112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>91</v>
       </c>
@@ -11153,7 +11153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>91</v>
       </c>
@@ -11194,7 +11194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>91</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>91</v>
       </c>
@@ -11276,7 +11276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>91</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>91</v>
       </c>
@@ -11358,7 +11358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>91</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>91</v>
       </c>
@@ -11440,7 +11440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>91</v>
       </c>
@@ -11481,7 +11481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>91</v>
       </c>
@@ -11522,7 +11522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>91</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>91</v>
       </c>
@@ -11604,7 +11604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>91</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>91</v>
       </c>
@@ -11686,7 +11686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>91</v>
       </c>
@@ -11727,7 +11727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>91</v>
       </c>
@@ -11768,7 +11768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>91</v>
       </c>
@@ -11809,7 +11809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>91</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>91</v>
       </c>
@@ -11891,7 +11891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>91</v>
       </c>
@@ -11932,7 +11932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>91</v>
       </c>
@@ -11973,7 +11973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>91</v>
       </c>
@@ -12014,7 +12014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>91</v>
       </c>
@@ -12055,7 +12055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>91</v>
       </c>
@@ -12096,7 +12096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>91</v>
       </c>
@@ -12137,7 +12137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>91</v>
       </c>
@@ -12178,7 +12178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>91</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>91</v>
       </c>
@@ -12260,7 +12260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>91</v>
       </c>
@@ -12301,7 +12301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>91</v>
       </c>
@@ -12342,7 +12342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>91</v>
       </c>
@@ -12383,7 +12383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>91</v>
       </c>
@@ -12424,7 +12424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>91</v>
       </c>
@@ -12465,7 +12465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>91</v>
       </c>
@@ -12506,7 +12506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>91</v>
       </c>
@@ -12547,7 +12547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>91</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>91</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>91</v>
       </c>
@@ -12670,7 +12670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>91</v>
       </c>
@@ -12711,7 +12711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>91</v>
       </c>
@@ -12752,7 +12752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>91</v>
       </c>
@@ -12793,7 +12793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>91</v>
       </c>
@@ -12834,7 +12834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>91</v>
       </c>
@@ -12875,7 +12875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>91</v>
       </c>
@@ -12916,7 +12916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>91</v>
       </c>
@@ -12957,7 +12957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>91</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>91</v>
       </c>
@@ -13039,7 +13039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
       <c r="K240">
         <v>2</v>
       </c>
@@ -13062,7 +13062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="241" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M241" t="s">
         <v>102</v>
       </c>
@@ -13076,7 +13076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="242" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M242" t="s">
         <v>102</v>
       </c>
@@ -13090,7 +13090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="243" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M243" t="s">
         <v>102</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="13:18" x14ac:dyDescent="0.25">
+    <row r="244" spans="13:18" x14ac:dyDescent="0.2">
       <c r="M244" t="s">
         <v>102</v>
       </c>
@@ -13124,263 +13124,353 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="D1" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
       <c r="D13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
       <c r="D14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>68</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
       <c r="B17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="s">
         <v>105</v>
       </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
       <c r="D19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>87</v>
       </c>
       <c r="B23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
+      <c r="C24">
+        <v>18</v>
+      </c>
       <c r="D24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>96</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>98</v>
       </c>
       <c r="B28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>100</v>
       </c>
       <c r="B30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>101</v>
+      </c>
+      <c r="C31">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>